<commit_message>
pass charge table export test
</commit_message>
<xml_diff>
--- a/src/templates/ShippingTableTemplate.xlsx
+++ b/src/templates/ShippingTableTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\php\yii2exts\exts\48-yii2-charging\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA4BE9E-B5BC-4CE4-8A7E-402205B2E2AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E51592E-7F90-459F-B254-338759933C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="27885" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT" sheetId="1" r:id="rId1"/>
@@ -46,10 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lx2(H+W)Limit(CM)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Price</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -75,6 +71,10 @@
   </si>
   <si>
     <t>DPD</t>
+  </si>
+  <si>
+    <t>L+2(H+W)Limit(CM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:J158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -501,24 +501,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
@@ -542,15 +542,15 @@
         <v>2.79</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="4">
         <v>31.5</v>
@@ -574,15 +574,15 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4">
         <v>30</v>
@@ -606,7 +606,7 @@
         <v>3.49</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>